<commit_message>
Updated Table Properties.xlsx to reflect later changes. Added field TypeID to database documentation. Worksheet ready for full property insertion.
</commit_message>
<xml_diff>
--- a/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Properties Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Field Explanation" sheetId="2" r:id="rId1"/>
+    <sheet name="Types" sheetId="3" r:id="rId2"/>
+    <sheet name="Properties Table" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Grotti</t>
   </si>
@@ -76,14 +78,131 @@
     <t>72.04861,612.6984,14.71273</t>
   </si>
   <si>
-    <t>CREATE TABLE [Properties] ([ID] INTEGER  NOT NULL PRIMARY KEY AUTOINCREMENT,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] INTEGER  NOT NULL,[Staff] INTEGER DEFAULT '0' NOT NULL,[StaffCap] INTEGER DEFAULT '10' NOT NULL,[Cost] INTEGER  NOT NULL)</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>StaffCap</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>TypeID</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [Properties] ([ID] INTEGER  NOT NULL PRIMARY KEY AUTOINCREMENT,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] INTEGER  NOT NULL,[Staff] INTEGER DEFAULT '0' NOT NULL,[StaffCap] INTEGER DEFAULT '10' NOT NULL,[Cost] INTEGER  NOT NULL, [TypeID] INTEGER  NOT NULL)</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Must be LESS THAN 30 characters long, white spaces and tab inserts also count for the character count</t>
+  </si>
+  <si>
+    <t>Is used to identify the property against the user while in game.</t>
+  </si>
+  <si>
+    <t>Represents a set of 3D coordinates reflecting the property display position in game</t>
+  </si>
+  <si>
+    <t>The field is store a single line using the template [x],[y],[z], decimal places must be separated by a single dot</t>
+  </si>
+  <si>
+    <t>Eg.: 79.76576,801.2764,15.16314</t>
+  </si>
+  <si>
+    <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission]</t>
+  </si>
+  <si>
+    <t>Stored as a single integer value</t>
+  </si>
+  <si>
+    <t>Eg.: 101</t>
+  </si>
+  <si>
+    <t>Total current staff</t>
+  </si>
+  <si>
+    <t>Inclusive maximum value that can be assigned to the Staff field</t>
+  </si>
+  <si>
+    <t>Game capital required to change owned flag to true</t>
+  </si>
+  <si>
+    <t>Unsed when flag is already true</t>
+  </si>
+  <si>
+    <t>Refer to page Types for more info</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Showroom</t>
+  </si>
+  <si>
+    <t>Clothes Store</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Resturant</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Petrol Station</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>StaffIncome</t>
+  </si>
+  <si>
+    <t>N/D</t>
+  </si>
+  <si>
+    <t>0/0</t>
+  </si>
+  <si>
+    <t>500/1000</t>
+  </si>
+  <si>
+    <t>150/250</t>
+  </si>
+  <si>
+    <t>50/100</t>
+  </si>
+  <si>
+    <t>250/500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +240,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,13 +260,313 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="25">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -150,7 +575,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -161,6 +586,67 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,33 +952,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="105.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="18"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="14"/>
+    </row>
+  </sheetData>
+  <sheetProtection password="85FC" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>2</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>5</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <v>6</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>7</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <v>8</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>9</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34">
+        <v>10</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="85FC" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="29" style="5" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="5"/>
-    <col min="7" max="7" width="167.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="5" width="9.140625" style="5"/>
+    <col min="6" max="6" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="255.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -508,15 +1382,18 @@
       <c r="E2" s="4">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="7">
         <v>599999</v>
       </c>
-      <c r="G2" s="1" t="str">
-        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "',"&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Grotti','79.76576,801.2764,15.16314',101,0,10,599999);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "',"&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Grotti','79.76576,801.2764,15.16314',101,0,10,599999,1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -532,15 +1409,18 @@
       <c r="E3" s="4">
         <v>10</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="7">
         <v>399999</v>
       </c>
-      <c r="G3" s="1" t="str">
-        <f t="shared" ref="G3:G11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "',"&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Perseus','22.08282,805.9178,14.76683',100,0,10,399999);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H3:H11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "',"&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Perseus','22.08282,805.9178,14.76683',100,0,10,399999,2);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -556,15 +1436,16 @@
       <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="7">
         <v>10000</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="G4" s="4"/>
+      <c r="H4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Shodi','14.46907,944.1911,14.71485',100,0,10,10000);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Shodi','14.46907,944.1911,14.71485',100,0,10,10000,);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -580,15 +1461,16 @@
       <c r="E5" s="4">
         <v>10</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="7">
         <v>100000</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="G5" s="4"/>
+      <c r="H5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('SuperStar','18.07519,980.3729,15.64596',101,0,10,100000);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('SuperStar','18.07519,980.3729,15.64596',101,0,10,100000,);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -604,15 +1486,18 @@
       <c r="E6" s="4">
         <v>50</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="7">
         <v>250000</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Apartment Block','66.77424,968.6838,13.65716',100,0,50,250000);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Apartment Block','66.77424,968.6838,13.65716',100,0,50,250000,5);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -628,15 +1513,16 @@
       <c r="E7" s="4">
         <v>10</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="7">
         <v>100000</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="G7" s="4"/>
+      <c r="H7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('TerrOil','105.8526,1120.935,14.67003',100,0,10,100000);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('TerrOil','105.8526,1120.935,14.67003',100,0,10,100000,);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -652,15 +1538,16 @@
       <c r="E8" s="4">
         <v>100</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="7">
         <v>1000000</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G8" s="4"/>
+      <c r="H8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995',100,0,100,1000000);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995',100,0,100,1000000,);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -676,15 +1563,16 @@
       <c r="E9" s="4">
         <v>50</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="7">
         <v>15000000</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="G9" s="4"/>
+      <c r="H9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036',100,0,50,15000000);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036',100,0,50,15000000,);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -700,15 +1588,16 @@
       <c r="E10" s="4">
         <v>100</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="7">
         <v>250000</v>
       </c>
-      <c r="G10" s="1" t="str">
+      <c r="G10" s="4"/>
+      <c r="H10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Office Block','25.91283,589.9072,14.71847',100,0,100,250000);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Office Block','25.91283,589.9072,14.71847',100,0,100,250000,);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -724,12 +1613,15 @@
       <c r="E11" s="4">
         <v>50</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="7">
         <v>100000</v>
       </c>
-      <c r="G11" s="1" t="str">
+      <c r="G11" s="4">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost) VALUES ('Construction Site','72.04861,612.6984,14.71273',100,0,50,100000);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Construction Site','72.04861,612.6984,14.71273',100,0,50,100000,10);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed version scheme to 0.0.REV (0.0.0.REV) alpha release Added reference to System.Drawing Possibility to buy properties using action key ([E]- keyboard [LB] - controller, working 100%) with on-time sql update No environment checks made on buy action (money, player on foot, etc) Blip icon reflects ownership status Blip member added to Property class Updated field Flags to VARCHAR(3) Added random MISSION_COMPLETE_AUDIO when buying a Property
</commit_message>
<xml_diff>
--- a/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -99,9 +99,6 @@
     <t>TypeID</t>
   </si>
   <si>
-    <t>CREATE TABLE [Properties] ([ID] INTEGER  NOT NULL PRIMARY KEY AUTOINCREMENT,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] INTEGER  NOT NULL,[Staff] INTEGER DEFAULT '0' NOT NULL,[StaffCap] INTEGER DEFAULT '10' NOT NULL,[Cost] INTEGER  NOT NULL, [TypeID] INTEGER  NOT NULL)</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>250/500</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [Properties] ([ID] INTEGER  NOT NULL PRIMARY KEY AUTOINCREMENT,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] VARCHAR(3)  NOT NULL,[Staff] INTEGER DEFAULT '0' NOT NULL,[StaffCap] INTEGER DEFAULT '10' NOT NULL,[Cost] INTEGER  NOT NULL, [TypeID] INTEGER  NOT NULL)</t>
   </si>
 </sst>
 </file>
@@ -955,7 +955,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,20 +965,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="15"/>
       <c r="C2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,27 +993,27 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="15"/>
       <c r="C6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="15"/>
       <c r="C7" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,27 +1023,27 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="15"/>
       <c r="C10" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="15"/>
       <c r="C11" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,13 +1053,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,13 +1079,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1105,20 +1105,20 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,20 +1133,20 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="15"/>
       <c r="C26" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,13 +1184,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,10 +1198,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,10 +1209,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,10 +1220,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,10 +1231,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,10 +1242,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,10 +1253,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,10 +1264,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1275,10 +1275,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1308,10 +1308,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1324,9 +1324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1363,7 @@
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1389,8 +1389,8 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "',"&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Grotti','79.76576,801.2764,15.16314',101,0,10,599999,1);</v>
+        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Grotti','79.76576,801.2764,15.16314','101',0,10,599999,1);</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1415,10 +1415,6 @@
       <c r="G3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "',"&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Perseus','22.08282,805.9178,14.76683',100,0,10,399999,2);</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1440,10 +1436,6 @@
         <v>10000</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Shodi','14.46907,944.1911,14.71485',100,0,10,10000,);</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1465,10 +1457,6 @@
         <v>100000</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('SuperStar','18.07519,980.3729,15.64596',101,0,10,100000,);</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1492,10 +1480,6 @@
       <c r="G6" s="4">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Apartment Block','66.77424,968.6838,13.65716',100,0,50,250000,5);</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1517,10 +1501,6 @@
         <v>100000</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('TerrOil','105.8526,1120.935,14.67003',100,0,10,100000,);</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1542,10 +1522,6 @@
         <v>1000000</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995',100,0,100,1000000,);</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1567,10 +1543,6 @@
         <v>15000000</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036',100,0,50,15000000,);</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1592,10 +1564,6 @@
         <v>250000</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Office Block','25.91283,589.9072,14.71847',100,0,100,250000,);</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1618,10 +1586,6 @@
       </c>
       <c r="G11" s="4">
         <v>10</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, Type) VALUES ('Construction Site','72.04861,612.6984,14.71273',100,0,50,100000,10);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PropertyManagerForm partially finished, main core working 100% Big change to database check Table Properties.xlsx for more info Staff management functions finished, Hire, Fire, Up-front pay. (Salary still waiting for another thread)
</commit_message>
<xml_diff>
--- a/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Field Explanation" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>Grotti</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission]</t>
   </si>
   <si>
-    <t>Stored as a single integer value</t>
-  </si>
-  <si>
     <t>Eg.: 101</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t>Unsed when flag is already true</t>
   </si>
   <si>
-    <t>Refer to page Types for more info</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
     <t>Showroom</t>
   </si>
   <si>
@@ -171,28 +162,55 @@
     <t>ID</t>
   </si>
   <si>
-    <t>StaffIncome</t>
-  </si>
-  <si>
-    <t>N/D</t>
-  </si>
-  <si>
-    <t>0/0</t>
-  </si>
-  <si>
-    <t>500/1000</t>
-  </si>
-  <si>
-    <t>150/250</t>
-  </si>
-  <si>
-    <t>50/100</t>
-  </si>
-  <si>
-    <t>250/500</t>
-  </si>
-  <si>
-    <t>CREATE TABLE [Properties] ([ID] INTEGER  NOT NULL PRIMARY KEY AUTOINCREMENT,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] VARCHAR(3)  NOT NULL,[Staff] INTEGER DEFAULT '0' NOT NULL,[StaffCap] INTEGER DEFAULT '10' NOT NULL,[Cost] INTEGER  NOT NULL, [TypeID] INTEGER  NOT NULL)</t>
+    <t>IncomeMin</t>
+  </si>
+  <si>
+    <t>IncomeMax</t>
+  </si>
+  <si>
+    <t>StaffSal</t>
+  </si>
+  <si>
+    <t>StaffPay</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [Properties] ([ID] INTEGER  PRIMARY KEY AUTOINCREMENT NOT NULL,[Name] VARCHAR(30)  UNIQUE NOT NULL,[Location] VARCHAR(150)  UNIQUE NOT NULL,[Flags] VARCHAR(3)  NOT NULL,[Staff] INTEGER DEFAULT '''0''' NOT NULL,[StaffCap] INTEGER DEFAULT '''10''' NOT NULL,[Cost] INTEGER  NOT NULL,[IncomeMin] INTEGER DEFAULT '0' NOT NULL,[IncomeMax] INTEGER DEFAULT '0' NOT NULL,[StaffSal] INTEGER DEFAULT '0' NOT NULL,[StaffPay] INTEGER DEFAULT '0' NOT NULL,[Income] INTEGER DEFAULT '0' NOT NULL,[TypeID] INTEGER  NOT NULL);</t>
+  </si>
+  <si>
+    <t>Min income value for each staff member</t>
+  </si>
+  <si>
+    <t>Max income value for each staff member</t>
+  </si>
+  <si>
+    <t>Salary paid to every staff member before income calculation</t>
+  </si>
+  <si>
+    <t>If player can't met StaffSal * Staff, no income is calculated</t>
+  </si>
+  <si>
+    <t>Up front payment to hire a new staff member</t>
+  </si>
+  <si>
+    <t>Can be 0</t>
+  </si>
+  <si>
+    <t>Income to collect</t>
+  </si>
+  <si>
+    <t>This value is calculated like follows: Random(IncomeMin, IncomeMax) * Staff</t>
+  </si>
+  <si>
+    <t>Calculations run every minute</t>
+  </si>
+  <si>
+    <t>Refer to Types page</t>
+  </si>
+  <si>
+    <t>Stored as a 3 char string</t>
   </si>
 </sst>
 </file>
@@ -202,7 +220,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,14 +258,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +278,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -338,21 +356,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -468,7 +471,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -480,13 +483,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -496,51 +514,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -575,7 +548,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -603,35 +576,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -640,13 +607,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -952,14 +919,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="105.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1036,14 +1004,14 @@
       <c r="A10" s="11"/>
       <c r="B10" s="15"/>
       <c r="C10" s="12" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="15"/>
       <c r="C11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,7 +1027,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1085,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,14 +1079,14 @@
         <v>25</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,18 +1104,16 @@
         <v>27</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -1159,8 +1125,145 @@
       <c r="B28" s="24"/>
       <c r="C28" s="14"/>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="14"/>
+    </row>
   </sheetData>
-  <sheetProtection password="85FC" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1168,165 +1271,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="25" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="25"/>
+    <col min="3" max="3" width="10.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="13" style="25" customWidth="1"/>
+    <col min="5" max="5" width="49" style="25" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
-        <v>2</v>
-      </c>
-      <c r="B4" s="28" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
-        <v>3</v>
-      </c>
-      <c r="B5" s="28" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
+        <v>6</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
-        <v>4</v>
-      </c>
-      <c r="B6" s="28" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
-        <v>5</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>8</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
+        <v>9</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
-        <v>6</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
-        <v>7</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
-        <v>8</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
-        <v>9</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34">
-        <v>10</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>53</v>
-      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection password="85FC" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,12 +1445,13 @@
     <col min="2" max="2" width="29" style="5" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="5"/>
     <col min="6" max="6" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="100.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="11" width="13.85546875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="5"/>
+    <col min="13" max="13" width="100.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1359,14 +1470,29 @@
       <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1385,15 +1511,30 @@
       <c r="F2" s="7">
         <v>599999</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','101',0,10,599999,1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="str">
+        <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","&amp;L2&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','101',0,10,599999,0, 0, 0, 0, 0,1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1412,15 +1553,30 @@
       <c r="F3" s="7">
         <v>399999</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','100',0,10,399999,2);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","&amp;L3&amp;");"</f>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','100',0,10,399999,0, 0, 0, 0, 0,2);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1439,15 +1595,30 @@
       <c r="F4" s="7">
         <v>10000</v>
       </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="str">
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Shodi','14.46907,944.1911,14.71485','100',0,10,10000,0);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Shodi','14.46907,944.1911,14.71485','100',0,10,10000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1466,15 +1637,30 @@
       <c r="F5" s="7">
         <v>100000</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="str">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('SuperStar','18.07519,980.3729,15.64596','101',0,10,100000,0);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('SuperStar','18.07519,980.3729,15.64596','101',0,10,100000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1493,15 +1679,30 @@
       <c r="F6" s="7">
         <v>250000</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Apartment Block','66.77424,968.6838,13.65716','100',0,50,250000,5);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Apartment Block','66.77424,968.6838,13.65716','100',0,50,250000,0, 0, 0, 0, 0,5);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1520,15 +1721,30 @@
       <c r="F7" s="7">
         <v>100000</v>
       </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="str">
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('TerrOil','105.8526,1120.935,14.67003','100',0,10,100000,0);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('TerrOil','105.8526,1120.935,14.67003','100',0,10,100000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1547,15 +1763,30 @@
       <c r="F8" s="7">
         <v>1000000</v>
       </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="str">
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995','100',0,100,1000000,0);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995','100',0,100,1000000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1574,15 +1805,30 @@
       <c r="F9" s="7">
         <v>15000000</v>
       </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="str">
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036','100',0,50,15000000,0);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036','100',0,50,15000000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1601,15 +1847,30 @@
       <c r="F10" s="7">
         <v>250000</v>
       </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="str">
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Office Block','25.91283,589.9072,14.71847','100',0,100,250000,0);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Office Block','25.91283,589.9072,14.71847','100',0,100,250000,0, 0, 0, 0, 0,0);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1628,12 +1889,27 @@
       <c r="F11" s="7">
         <v>100000</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
         <v>10</v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, TypeID) VALUES ('Construction Site','72.04861,612.6984,14.71273','100',0,50,100000,10);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Construction Site','72.04861,612.6984,14.71273','100',0,50,100000,0, 0, 0, 0, 0,10);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor change to Table Properties.xlsx
</commit_message>
<xml_diff>
--- a/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>Grotti</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Stored as a 3 char string</t>
+  </si>
+  <si>
+    <t>LEAVE AT 0</t>
   </si>
 </sst>
 </file>
@@ -922,7 +925,7 @@
   <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1238,9 @@
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="24"/>
-      <c r="C44" s="14"/>
+      <c r="C44" s="14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">

</xml_diff>

<commit_message>
Added flag ShowBlip to disable on map blip display.
</commit_message>
<xml_diff>
--- a/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
+++ b/ ultimate-business-mod/UltimateBusinessMod/Development Data/Database/Table Properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Field Explanation" sheetId="2" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Eg.: 79.76576,801.2764,15.16314</t>
   </si>
   <si>
-    <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission]</t>
-  </si>
-  <si>
     <t>Eg.: 101</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>LEAVE AT 0</t>
+  </si>
+  <si>
+    <t>Used as 'bulk storage' for the boolean variables [Ownable][Owned][ContextMission][ShowBlip]</t>
   </si>
 </sst>
 </file>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,21 +1000,21 @@
         <v>22</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="15"/>
       <c r="C10" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="15"/>
       <c r="C11" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,14 +1082,14 @@
         <v>25</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="15"/>
       <c r="C22" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1107,10 +1107,10 @@
         <v>27</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,17 +1159,17 @@
         <v>27</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="15"/>
       <c r="C34" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,17 +1187,17 @@
         <v>27</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="15"/>
       <c r="C38" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,31 +1215,31 @@
         <v>27</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="15"/>
       <c r="C42" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="15"/>
       <c r="C43" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="24"/>
       <c r="C44" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>26</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>20</v>
@@ -1309,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -1331,7 +1331,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1342,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
@@ -1353,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
@@ -1364,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
@@ -1375,7 +1375,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
@@ -1386,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -1408,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
@@ -1439,9 +1439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M2:M11"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,25 +1476,25 @@
         <v>25</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="4">
-        <v>101</v>
+        <v>1011</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="M2" s="1" t="str">
         <f>"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A2&amp;"','" &amp;B2&amp; "','"&amp;C2&amp;"',"&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;","&amp;L2&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','101',0,10,599999,0, 0, 0, 0, 0,1);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Grotti','79.76576,801.2764,15.16314','1011',0,10,599999,0, 0, 0, 0, 0,1);</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="4">
-        <v>100</v>
+        <v>1002</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="M3" s="1" t="str">
         <f t="shared" ref="M3:M11" si="0">"INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('" &amp;A3&amp;"','" &amp;B3&amp; "','"&amp;C3&amp;"',"&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;","&amp;L3&amp;");"</f>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','100',0,10,399999,0, 0, 0, 0, 0,2);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Perseus','22.08282,805.9178,14.76683','1002',0,10,399999,0, 0, 0, 0, 0,2);</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="M4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Shodi','14.46907,944.1911,14.71485','100',0,10,10000,0, 0, 0, 0, 0,0);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Shodi','14.46907,944.1911,14.71485','1001',0,10,10000,0, 0, 0, 0, 0,0);</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1631,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="4">
-        <v>101</v>
+        <v>1011</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('SuperStar','18.07519,980.3729,15.64596','101',0,10,100000,0, 0, 0, 0, 0,0);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('SuperStar','18.07519,980.3729,15.64596','1011',0,10,100000,0, 0, 0, 0, 0,0);</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1673,7 +1673,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Apartment Block','66.77424,968.6838,13.65716','100',0,50,250000,0, 0, 0, 0, 0,5);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Apartment Block','66.77424,968.6838,13.65716','1001',0,50,250000,0, 0, 0, 0, 0,5);</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('TerrOil','105.8526,1120.935,14.67003','100',0,10,100000,0, 0, 0, 0, 0,0);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('TerrOil','105.8526,1120.935,14.67003','1001',0,10,100000,0, 0, 0, 0, 0,0);</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995','100',0,100,1000000,0, 0, 0, 0, 0,0);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Liberty City Delivery','-24.0677,880.597,18.74995','1001',0,100,1000000,0, 0, 0, 0, 0,0);</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036','100',0,50,15000000,0, 0, 0, 0, 0,0);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('The Libertonian Museum','-86.32443,821.8265,18.63036','1001',0,50,15000000,0, 0, 0, 0, 0,0);</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Office Block','25.91283,589.9072,14.71847','100',0,100,250000,0, 0, 0, 0, 0,0);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Office Block','25.91283,589.9072,14.71847','1001',0,100,250000,0, 0, 0, 0, 0,0);</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1883,7 +1883,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="4">
-        <v>100</v>
+        <v>1001</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Construction Site','72.04861,612.6984,14.71273','100',0,50,100000,0, 0, 0, 0, 0,10);</v>
+        <v>INSERT OR IGNORE INTO Properties (Name, Location, Flags, Staff, StaffCap, Cost, IncomeMin, IncomeMax, StaffSal, StaffPay, Income, TypeID) VALUES ('Construction Site','72.04861,612.6984,14.71273','1001',0,50,100000,0, 0, 0, 0, 0,10);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>